<commit_message>
Fully functional network graph
</commit_message>
<xml_diff>
--- a/network_input.xlsx
+++ b/network_input.xlsx
@@ -138,7 +138,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,7 +419,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B2" sqref="B2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -506,7 +506,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>